<commit_message>
Keeping it up to date
</commit_message>
<xml_diff>
--- a/Dr. E Nduati, Superviser/Research_Report_Evaluation_Rubric.xlsx
+++ b/Dr. E Nduati, Superviser/Research_Report_Evaluation_Rubric.xlsx
@@ -1,23 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BSc Research Project\Research Project M&amp;E - 2020_2021\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\STUDY\4.GIS\G I S 4.2\0.Project\Dr. E Nduati, Superviser\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92CA408B-AC25-4E5C-A93E-1202BD52DBE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rubric" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -26,9 +34,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
-    <t>Name: Stildon Kimani Marigi</t>
-  </si>
-  <si>
     <t>Marks</t>
   </si>
   <si>
@@ -153,12 +158,15 @@
   </si>
   <si>
     <t xml:space="preserve">Title: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name: </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -223,9 +231,6 @@
   </cellStyleXfs>
   <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
@@ -254,6 +259,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -535,11 +543,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C48"/>
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -550,330 +558,330 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="3" t="s">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="9"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="10"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="10" t="s">
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="10" t="s">
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="10" t="s">
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="10"/>
-      <c r="C16" s="10"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="10" t="s">
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="10" t="s">
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="9"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="10"/>
-      <c r="C18" s="10"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="10"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="10"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="s">
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="10"/>
-      <c r="C20" s="10"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="10" t="s">
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B21" s="10"/>
-      <c r="C21" s="10"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="10" t="s">
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B22" s="10"/>
-      <c r="C22" s="10"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="10" t="s">
+      <c r="B23" s="9"/>
+      <c r="C23" s="9"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B23" s="10"/>
-      <c r="C23" s="10"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="10" t="s">
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B24" s="10"/>
-      <c r="C24" s="10"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="10" t="s">
+      <c r="B25" s="9"/>
+      <c r="C25" s="9"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="9"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B25" s="10"/>
-      <c r="C25" s="10"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="10"/>
-      <c r="B26" s="10"/>
-      <c r="C26" s="10"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="9" t="s">
+      <c r="B27" s="9"/>
+      <c r="C27" s="9"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B27" s="10"/>
-      <c r="C27" s="10"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="10" t="s">
+      <c r="B28" s="9"/>
+      <c r="C28" s="9"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B28" s="10"/>
-      <c r="C28" s="10"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="10" t="s">
+      <c r="B29" s="9"/>
+      <c r="C29" s="9"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B29" s="10"/>
-      <c r="C29" s="10"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="10" t="s">
+      <c r="B30" s="9"/>
+      <c r="C30" s="9"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B30" s="10"/>
-      <c r="C30" s="10"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="10" t="s">
+      <c r="B31" s="9"/>
+      <c r="C31" s="9"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B31" s="10"/>
-      <c r="C31" s="10"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="10" t="s">
+      <c r="B32" s="9"/>
+      <c r="C32" s="9"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="5"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B32" s="10"/>
-      <c r="C32" s="10"/>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="6"/>
-      <c r="B33" s="6"/>
-      <c r="C33" s="6"/>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
+      <c r="B34" s="4"/>
+      <c r="C34" s="4"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B34" s="5"/>
-      <c r="C34" s="5"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="5" t="s">
+      <c r="B35" s="4"/>
+      <c r="C35" s="4"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B35" s="5"/>
-      <c r="C35" s="5"/>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="5" t="s">
+      <c r="B36" s="4"/>
+      <c r="C36" s="4"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B36" s="5"/>
-      <c r="C36" s="5"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="5" t="s">
+      <c r="B37" s="4"/>
+      <c r="C37" s="4"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B37" s="5"/>
-      <c r="C37" s="5"/>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="5" t="s">
+      <c r="B38" s="4"/>
+      <c r="C38" s="4"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B38" s="5"/>
-      <c r="C38" s="5"/>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="5" t="s">
+      <c r="B39" s="4"/>
+      <c r="C39" s="4"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="5"/>
+      <c r="B40" s="5"/>
+      <c r="C40" s="5"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B39" s="5"/>
-      <c r="C39" s="5"/>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="6"/>
-      <c r="B40" s="6"/>
-      <c r="C40" s="6"/>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="4" t="s">
+      <c r="B41" s="4"/>
+      <c r="C41" s="4"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B41" s="5"/>
-      <c r="C41" s="5"/>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="5" t="s">
+      <c r="B42" s="4"/>
+      <c r="C42" s="4"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B42" s="5"/>
-      <c r="C42" s="5"/>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="5" t="s">
+      <c r="B43" s="4"/>
+      <c r="C43" s="4"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B43" s="5"/>
-      <c r="C43" s="5"/>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="5" t="s">
+      <c r="B44" s="4"/>
+      <c r="C44" s="4"/>
+    </row>
+    <row r="45" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B44" s="5"/>
-      <c r="C44" s="5"/>
-    </row>
-    <row r="45" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A45" s="5" t="s">
+      <c r="B45" s="4"/>
+      <c r="C45" s="4"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B45" s="5"/>
-      <c r="C45" s="5"/>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="5" t="s">
+      <c r="B46" s="4"/>
+      <c r="C46" s="4"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="4"/>
+      <c r="B47" s="4"/>
+      <c r="C47" s="4"/>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B46" s="5"/>
-      <c r="C46" s="5"/>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="5"/>
-      <c r="B47" s="5"/>
-      <c r="C47" s="5"/>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="B48" s="8"/>
-      <c r="C48" s="8"/>
+      <c r="B48" s="7"/>
+      <c r="C48" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>